<commit_message>
Added functionality of finding differential elevations from a specified point and overlaying another source's elevation data
</commit_message>
<xml_diff>
--- a/Plots and Data/MajorPoints.xlsx
+++ b/Plots and Data/MajorPoints.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\Spring2018\EWB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srija\Desktop\EWB-Elevation-Analysis-Toolkit\Plots and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0137E89-2331-4765-A2FB-93B6FD31B77F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +108,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,8 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,23 +457,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -495,14 +500,14 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>2.3292809999999999</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>33.2532</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -512,14 +517,14 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>2.3360810000000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>33.253700000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -529,14 +534,14 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>2.326581</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>33.245100000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -546,14 +551,14 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>2.3197390000000002</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>33.246000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -563,14 +568,14 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>2.3403499999999999</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>33.254600000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -580,14 +585,14 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>2.324389</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>33.259500000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -596,6 +601,12 @@
       </c>
       <c r="C8" t="s">
         <v>25</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.3196888900000001</v>
+      </c>
+      <c r="E8" s="1">
+        <v>33.248888890000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>